<commit_message>
case b - heatsink script
</commit_message>
<xml_diff>
--- a/FE12/Cell Cooling/Accumulator Cooling Outline.xlsx
+++ b/FE12/Cell Cooling/Accumulator Cooling Outline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\OneDrive - University of California, Davis\Documents\GitHub\FE12-Accumulator\FE12\Cell Cooling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB00C3F4-9A40-45C5-A205-A73FE6A9BA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8662AB75-9603-4CAF-B829-D75B2E4B8F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{AEF49FB0-9177-41FE-B695-70313FA2271C}"/>
+    <workbookView xWindow="7200" yWindow="4020" windowWidth="21600" windowHeight="12465" xr2:uid="{AEF49FB0-9177-41FE-B695-70313FA2271C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Note: Scale off RMS power, or speed if we have that estimate, Current is 3p for ECM</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Max Q (Ohmic Heating) (kW)</t>
+  </si>
+  <si>
+    <t>Current</t>
   </si>
 </sst>
 </file>
@@ -242,12 +245,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C75DC4B-318F-4CDE-AE7F-1B47732BB2AC}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,7 +697,7 @@
         <v>18.25</v>
       </c>
       <c r="F4">
-        <f>K11</f>
+        <f>K12</f>
         <v>20</v>
       </c>
       <c r="G4">
@@ -718,159 +722,152 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B5">
-        <f>(B4*1000/4/3.85)^2*J19/1000</f>
-        <v>10.688986338336989</v>
-      </c>
-      <c r="C5">
-        <f>(C4*1000/4/3.85)^2*J19/1000</f>
-        <v>13.760488699612077</v>
-      </c>
-      <c r="D5">
-        <f>(D4*1000/4/3.85)^2*J19/1000</f>
-        <v>17.219387755102037</v>
-      </c>
-      <c r="E5">
-        <f>(E4*1000/4/3.85)^2*J19/1000</f>
-        <v>21.065683504806877</v>
-      </c>
-      <c r="F5">
-        <f>(F4*1000/4/3.85)^2*J19/1000</f>
-        <v>25.299375948726592</v>
-      </c>
-      <c r="G5">
-        <f>(G4*1000/4/3.85)^2*J19</f>
-        <v>29920.465086861186</v>
-      </c>
+        <f>B4/504*1000</f>
+        <v>25.793650793650791</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" t="s">
-        <v>21</v>
+        <v>45</v>
+      </c>
+      <c r="G6">
+        <f>(G4*1000/4/3.85)^2*J20</f>
+        <v>29920.465086861186</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J8" s="2">
-        <v>457.76</v>
-      </c>
-      <c r="K8" s="2">
-        <v>30.64</v>
-      </c>
-      <c r="L8" s="2">
-        <v>13.56</v>
-      </c>
-      <c r="M8" s="3">
-        <v>40</v>
+        <v>22</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="2">
+        <v>457.76</v>
+      </c>
+      <c r="K9" s="2">
+        <v>30.64</v>
+      </c>
+      <c r="L9" s="2">
+        <v>13.56</v>
+      </c>
+      <c r="M9" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H10" s="4" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J11" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" t="s">
-        <v>31</v>
-      </c>
-      <c r="K11">
-        <v>20</v>
-      </c>
-      <c r="L11" t="s">
-        <v>32</v>
-      </c>
-      <c r="M11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="K12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="L12" t="s">
         <v>32</v>
       </c>
-      <c r="M12">
-        <v>16.5</v>
+      <c r="M12" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13">
+        <v>13</v>
+      </c>
+      <c r="L13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M13">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J14" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J18" t="s">
+    <row r="19" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J19">
+    <row r="20" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J20">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J21" t="s">
+    <row r="22" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J22" s="3">
+    <row r="23" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J23" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J24" t="s">
+    <row r="25" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J25">
+    <row r="26" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J26">
         <v>30</v>
       </c>
     </row>
@@ -880,6 +877,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEB6A5575DD73B409EDC833CB0FB3305" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7580991daa6a3ab96ec158cd6f4c0033">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6c1e9144-75e6-4a9b-92e6-42d0d80c008e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e8f8a99fd8fca58167c486dffa4ecf7d" ns3:_="">
     <xsd:import namespace="6c1e9144-75e6-4a9b-92e6-42d0d80c008e"/>
@@ -1067,22 +1079,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED011950-3B00-40BA-9447-680D8BBD1527}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4351E797-52B9-45EB-871E-EE9B7E095236}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{836D7157-30DA-4DD7-B7E2-00BFDB1FF1E6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1098,21 +1112,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4351E797-52B9-45EB-871E-EE9B7E095236}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED011950-3B00-40BA-9447-680D8BBD1527}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>